<commit_message>
added manual testing docs
</commit_message>
<xml_diff>
--- a/TestData/EmailData.xlsx
+++ b/TestData/EmailData.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="32">
   <si>
     <t>1@##@gmailcom.com</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Expected Launch : Dec 2026</t>
+  </si>
+  <si>
+    <t>Expected Launch : Mar 2026</t>
   </si>
 </sst>
 </file>
@@ -589,7 +592,7 @@
         <v>15</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
@@ -600,7 +603,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
added e.getMessage() for testcases
</commit_message>
<xml_diff>
--- a/TestData/EmailData.xlsx
+++ b/TestData/EmailData.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="37">
   <si>
     <t>1@##@gmailcom.com</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>Expected Launch : Feb 2026</t>
+  </si>
+  <si>
+    <t>2026 Yamaha MT-03</t>
+  </si>
+  <si>
+    <t>2026 Yamaha R3</t>
   </si>
 </sst>
 </file>
@@ -617,7 +623,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>20</v>
@@ -639,7 +645,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>25</v>

</xml_diff>

<commit_message>
Done with Selenium Grid
</commit_message>
<xml_diff>
--- a/TestData/EmailData.xlsx
+++ b/TestData/EmailData.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="88">
   <si>
     <t>1@##@gmailcom.com</t>
   </si>
@@ -149,6 +149,159 @@
   </si>
   <si>
     <t>2026 Yamaha R3</t>
+  </si>
+  <si>
+    <t>2026 Hero Mavrick 440</t>
+  </si>
+  <si>
+    <t>Rs. 2.30 Lakh</t>
+  </si>
+  <si>
+    <t>Royal Enfield Bullet 650</t>
+  </si>
+  <si>
+    <t>Rs. 3.40 Lakh</t>
+  </si>
+  <si>
+    <t>Triumph Speed 350</t>
+  </si>
+  <si>
+    <t>Rs. 1.90 Lakh</t>
+  </si>
+  <si>
+    <t>FB Mondial Piega 452</t>
+  </si>
+  <si>
+    <t>Rs. 5.00 Lakh</t>
+  </si>
+  <si>
+    <t>2026 Bajaj Pulsar</t>
+  </si>
+  <si>
+    <t>Rs. 95,000</t>
+  </si>
+  <si>
+    <t>BMW F 450 GS</t>
+  </si>
+  <si>
+    <t>Rs. 4.50 Lakh</t>
+  </si>
+  <si>
+    <t>Hero Karizma XMR 250</t>
+  </si>
+  <si>
+    <t>Rs. 2.00 Lakh</t>
+  </si>
+  <si>
+    <t>2026 Husqvarna Svartpilen 401</t>
+  </si>
+  <si>
+    <t>Rs. 2.99 Lakh</t>
+  </si>
+  <si>
+    <t>2026 Husqvarna Vitpilen 250</t>
+  </si>
+  <si>
+    <t>Royal Enfield Flying Flea C6</t>
+  </si>
+  <si>
+    <t>Kawasaki W230</t>
+  </si>
+  <si>
+    <t>Rs. 1.50 Lakh</t>
+  </si>
+  <si>
+    <t>Expected Launch : Apr 2026</t>
+  </si>
+  <si>
+    <t>2026 Yezdi Scrambler</t>
+  </si>
+  <si>
+    <t>Rs. 2.15 Lakh</t>
+  </si>
+  <si>
+    <t>BSA Scrambler</t>
+  </si>
+  <si>
+    <t>Rs. 3.45 Lakh</t>
+  </si>
+  <si>
+    <t>BSA Electric Bike</t>
+  </si>
+  <si>
+    <t>Rs. 2.50 Lakh</t>
+  </si>
+  <si>
+    <t>Triumph Bonneville 350</t>
+  </si>
+  <si>
+    <t>Rs. 1.85 Lakh</t>
+  </si>
+  <si>
+    <t>2026 KTM RC 390</t>
+  </si>
+  <si>
+    <t>Rs. 3.50 Lakh</t>
+  </si>
+  <si>
+    <t>Bajaj Platina 125</t>
+  </si>
+  <si>
+    <t>Rs. 80,000</t>
+  </si>
+  <si>
+    <t>Bajaj Pulsar NS150</t>
+  </si>
+  <si>
+    <t>Rs. 1.22 Lakh</t>
+  </si>
+  <si>
+    <t>BSA Bantam 350</t>
+  </si>
+  <si>
+    <t>Rs. 2.20 Lakh</t>
+  </si>
+  <si>
+    <t>Expected Launch : Jul 2026</t>
+  </si>
+  <si>
+    <t>KTM 350 Duke</t>
+  </si>
+  <si>
+    <t>Rs. 2.60 Lakh</t>
+  </si>
+  <si>
+    <t>Ola Cruiser</t>
+  </si>
+  <si>
+    <t>Rs. 2.70 Lakh</t>
+  </si>
+  <si>
+    <t>Expected Launch : Aug 2026</t>
+  </si>
+  <si>
+    <t>Royal Enfield 250</t>
+  </si>
+  <si>
+    <t>Rs. 1.30 Lakh</t>
+  </si>
+  <si>
+    <t>Expected Launch : Sep 2026</t>
+  </si>
+  <si>
+    <t>Royal Enfield Interceptor 750</t>
+  </si>
+  <si>
+    <t>Rs. 3.80 Lakh</t>
+  </si>
+  <si>
+    <t>Expected Launch : Nov 2026</t>
+  </si>
+  <si>
+    <t>KTM Duke 490</t>
+  </si>
+  <si>
+    <t>Rs. 4.00 Lakh</t>
   </si>
 </sst>
 </file>
@@ -575,7 +728,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D08465B5-2025-4D19-9577-739F89D91275}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="A2:C8"/>
@@ -601,10 +754,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>31</v>
@@ -612,21 +765,21 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>21</v>
@@ -634,10 +787,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>21</v>
@@ -645,10 +798,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>21</v>
@@ -656,24 +809,255 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>